<commit_message>
learnt about inserting data/ primary key, defaults
</commit_message>
<xml_diff>
--- a/SQL-Commands.xlsx
+++ b/SQL-Commands.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23219"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23223"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2B420C8-0557-42CD-B8A8-F8775D400F25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C624321-2956-4014-B91D-C323D08ED032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SQL" sheetId="1" r:id="rId1"/>
+    <sheet name="SQL - Basic Commands" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -25,71 +25,113 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>SQL Commands</t>
   </si>
   <si>
+    <t>CLI Commands</t>
+  </si>
+  <si>
+    <t>DATABASE</t>
+  </si>
+  <si>
+    <t>TABLE</t>
+  </si>
+  <si>
+    <t>INSERT</t>
+  </si>
+  <si>
+    <t>set sql_mode='';</t>
+  </si>
+  <si>
     <t>// start the CLI</t>
   </si>
   <si>
     <t>// create table mentioning column data types</t>
   </si>
   <si>
+    <t>// insert data into particular table with specified column</t>
+  </si>
+  <si>
     <t>mysql-ctl cli;</t>
   </si>
   <si>
-    <t>create table &lt;table_name&gt;</t>
-  </si>
-  <si>
-    <t>(</t>
+    <t>// provide default values for columns if column values not specified</t>
+  </si>
+  <si>
+    <t>// the order matters</t>
+  </si>
+  <si>
+    <t>show warnings;</t>
+  </si>
+  <si>
+    <t>// not null says value cant hold null on insert or CRUD</t>
+  </si>
+  <si>
+    <t>insert into &lt;table_name&gt;(colA, colB...colN)</t>
   </si>
   <si>
     <t>// lists the current database exists in mySQL server</t>
   </si>
   <si>
-    <t>column_name data_type,</t>
+    <t xml:space="preserve">// primary key are unique identifiers </t>
+  </si>
+  <si>
+    <t>values ('r1-colAVal', r1-colBVal...valN), ('r2-colAVal', r2-colBVal...valN), ...N;</t>
   </si>
   <si>
     <t>show databases;</t>
   </si>
   <si>
-    <t>column_name data_type</t>
+    <t>create table &lt;table_name&gt; (</t>
+  </si>
+  <si>
+    <t>column_name data_type not null default value auto_increment,</t>
+  </si>
+  <si>
+    <t>// if default value provided for all columns</t>
+  </si>
+  <si>
+    <t>// create database followed by given name</t>
+  </si>
+  <si>
+    <t>column_name data_type not null default value,</t>
+  </si>
+  <si>
+    <t>insert into &lt;table_name&gt;() values();</t>
+  </si>
+  <si>
+    <t>create database &lt;database_name&gt;;</t>
+  </si>
+  <si>
+    <t>primary key (col_name)</t>
   </si>
   <si>
     <t>);</t>
   </si>
   <si>
-    <t>// create database followed by given name</t>
-  </si>
-  <si>
-    <t>create database &lt;database_name&gt;;</t>
+    <t>// deleting created database (careful with this command)</t>
   </si>
   <si>
     <t>// lists the current table in particular database</t>
   </si>
   <si>
+    <t>drop database &lt;database_name&gt;;</t>
+  </si>
+  <si>
     <t>show tables;</t>
   </si>
   <si>
-    <t>// deleting created database (careful with this command)</t>
-  </si>
-  <si>
-    <t>drop database &lt;database_name&gt;;</t>
-  </si>
-  <si>
     <t>// lists the current columns in particular table</t>
   </si>
   <si>
+    <t>// to work with specific database</t>
+  </si>
+  <si>
     <t>show columns from &lt;table_name&gt;;</t>
   </si>
   <si>
-    <t>// to work with specific database</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
     <t>use &lt;database_name&gt;;</t>
   </si>
   <si>
@@ -106,13 +148,22 @@
   </si>
   <si>
     <t>drop table &lt;table_name&gt;;</t>
+  </si>
+  <si>
+    <t>VIEW</t>
+  </si>
+  <si>
+    <t>// to view data in any given table</t>
+  </si>
+  <si>
+    <t>select * from &lt;table_name&gt;;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +196,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -160,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -177,11 +235,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -193,6 +332,31 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,161 +671,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E20"/>
+  <dimension ref="B2:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="58.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="58.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="3.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="85.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:9">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="5" t="s">
+      <c r="I2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="6" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="20" t="s">
         <v>4</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="7"/>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
+      <c r="G5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
+      <c r="G6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="12"/>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
+      <c r="G7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="7"/>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
+      <c r="G8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="5" t="s">
-        <v>11</v>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="12"/>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>13</v>
+      <c r="G10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="7"/>
+      <c r="G11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="5" t="s">
-        <v>15</v>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="12"/>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>17</v>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>20</v>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="12"/>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="6" t="s">
-        <v>21</v>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="8"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="13"/>
       <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>26</v>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
learnt about crud op in mysql
</commit_message>
<xml_diff>
--- a/SQL-Commands.xlsx
+++ b/SQL-Commands.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23229"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C624321-2956-4014-B91D-C323D08ED032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25582D95-678A-4F29-8BA2-3017B4307604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>SQL Commands</t>
   </si>
@@ -78,7 +78,7 @@
     <t xml:space="preserve">// primary key are unique identifiers </t>
   </si>
   <si>
-    <t>values ('r1-colAVal', r1-colBVal...valN), ('r2-colAVal', r2-colBVal...valN), ...N;</t>
+    <t>values ('r1-colAVal', r1-colBVal...valN),</t>
   </si>
   <si>
     <t>show databases;</t>
@@ -87,30 +87,42 @@
     <t>create table &lt;table_name&gt; (</t>
   </si>
   <si>
+    <t>('r2-colAVal', r2-colBVal...valN),</t>
+  </si>
+  <si>
+    <t>drop primary key</t>
+  </si>
+  <si>
+    <t>alter</t>
+  </si>
+  <si>
     <t>column_name data_type not null default value auto_increment,</t>
   </si>
   <si>
+    <t>(...N);</t>
+  </si>
+  <si>
+    <t>// create database followed by given name</t>
+  </si>
+  <si>
+    <t>column_name data_type not null default value primary key,</t>
+  </si>
+  <si>
+    <t>create database &lt;database_name&gt;;</t>
+  </si>
+  <si>
+    <t>primary key (col_name)</t>
+  </si>
+  <si>
     <t>// if default value provided for all columns</t>
   </si>
   <si>
-    <t>// create database followed by given name</t>
-  </si>
-  <si>
-    <t>column_name data_type not null default value,</t>
+    <t>);</t>
   </si>
   <si>
     <t>insert into &lt;table_name&gt;() values();</t>
   </si>
   <si>
-    <t>create database &lt;database_name&gt;;</t>
-  </si>
-  <si>
-    <t>primary key (col_name)</t>
-  </si>
-  <si>
-    <t>);</t>
-  </si>
-  <si>
     <t>// deleting created database (careful with this command)</t>
   </si>
   <si>
@@ -150,20 +162,89 @@
     <t>drop table &lt;table_name&gt;;</t>
   </si>
   <si>
+    <t>l</t>
+  </si>
+  <si>
     <t>VIEW</t>
   </si>
   <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
     <t>// to view data in any given table</t>
   </si>
   <si>
+    <t>// * gives all columns</t>
+  </si>
+  <si>
+    <t>WITH WHERE / SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WITH WHERE </t>
+  </si>
+  <si>
+    <t>// or can list out needed columns by &lt;column_name&gt;</t>
+  </si>
+  <si>
+    <t>// Try selecting before any update action</t>
+  </si>
+  <si>
+    <t>// Try selecting before any delete action</t>
+  </si>
+  <si>
     <t>select * from &lt;table_name&gt;;</t>
+  </si>
+  <si>
+    <t>update &lt;table_name&gt; set &lt;column_name&gt; = &lt;new_value&gt;, &lt;column_name&gt; = &lt;new_value&gt;</t>
+  </si>
+  <si>
+    <t>delete from &lt;table_name&gt; where &lt;column_name&gt; = &lt;column_value&gt;;</t>
+  </si>
+  <si>
+    <t>// select expression (with any order)</t>
+  </si>
+  <si>
+    <t>where &lt;column_name&gt; = &lt;old_value&gt;;</t>
+  </si>
+  <si>
+    <t>select &lt;colA&gt;, &lt;colB&gt; from &lt;table_name&gt;;</t>
+  </si>
+  <si>
+    <t>// Deleting records/enties from the table</t>
+  </si>
+  <si>
+    <t>delete from &lt;table_name&gt;;</t>
+  </si>
+  <si>
+    <t>// select on column conditions with where which returs one or more values</t>
+  </si>
+  <si>
+    <t>// column values are case in-sensitive, it deals with case</t>
+  </si>
+  <si>
+    <t>select * from &lt;table_name&gt; where &lt;col_name&gt; operator value;</t>
+  </si>
+  <si>
+    <t>select * from &lt;table_name&gt; where &lt;col_name&gt; operator &lt;col_name&gt;;</t>
+  </si>
+  <si>
+    <t>WITH ALIASES</t>
+  </si>
+  <si>
+    <t>// usefull when joining tables</t>
+  </si>
+  <si>
+    <t>select &lt;col_name&gt; as &lt;aliase_name&gt; from &lt;table_name&gt;;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,15 +271,46 @@
       <name val="Consolas"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0D0D0D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF808080"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -316,11 +428,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -329,34 +456,50 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,19 +814,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I41"/>
+  <dimension ref="B2:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="58.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="71.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="4" max="4" width="83.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="85.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" style="1" customWidth="1"/>
@@ -691,54 +834,54 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:10">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:10">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="2:9">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:10">
+      <c r="B4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="20" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="31" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:10">
+      <c r="B5" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
       <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="2:10">
+      <c r="B6" s="20" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
       <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
@@ -746,212 +889,327 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="12"/>
+    <row r="7" spans="2:10">
+      <c r="B7" s="8"/>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="6"/>
+      <c r="G7" s="27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:10">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="G8" s="6" t="s">
+      <c r="E8" s="6"/>
+      <c r="G8" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="2:10">
+      <c r="B9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="12"/>
-      <c r="D10" s="3" t="s">
+      <c r="E9" s="6"/>
+      <c r="G9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="G10" s="5" t="s">
+      <c r="I9" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="10" t="s">
+      <c r="J9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="3" t="s">
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="8"/>
+      <c r="D10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="G11" s="6" t="s">
+      <c r="E10" s="6"/>
+      <c r="G10" s="27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="11" t="s">
+    <row r="11" spans="2:10">
+      <c r="B11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="12"/>
-      <c r="D13" s="1" t="s">
+      <c r="E11" s="6"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="B14" s="10" t="s">
+      <c r="D12" s="24" t="s">
         <v>28</v>
       </c>
+      <c r="E12" s="6"/>
+      <c r="G12" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="8"/>
+      <c r="D13" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="G13" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="12"/>
+        <v>33</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="8"/>
       <c r="D16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="13"/>
-      <c r="E19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="10" t="s">
+      <c r="E16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="D17" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="18"/>
+      <c r="E19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="6" t="s">
+      <c r="E20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="7"/>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="7"/>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="8"/>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="6"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="G26" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="G27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="G28" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="G30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="7"/>
+      <c r="E31" s="6"/>
+      <c r="G31" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="7"/>
+      <c r="E37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="15"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
learnt about string functions in mysql
</commit_message>
<xml_diff>
--- a/SQL-Commands.xlsx
+++ b/SQL-Commands.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23308"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25582D95-678A-4F29-8BA2-3017B4307604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2931A1A7-71FD-4E1C-9CA8-2B41112CD492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>SQL Commands</t>
   </si>
@@ -108,6 +108,9 @@
     <t>column_name data_type not null default value primary key,</t>
   </si>
   <si>
+    <t>rename table books to books_store;</t>
+  </si>
+  <si>
     <t>create database &lt;database_name&gt;;</t>
   </si>
   <si>
@@ -162,9 +165,6 @@
     <t>drop table &lt;table_name&gt;;</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
     <t>VIEW</t>
   </si>
   <si>
@@ -238,6 +238,63 @@
   </si>
   <si>
     <t>select &lt;col_name&gt; as &lt;aliase_name&gt; from &lt;table_name&gt;;</t>
+  </si>
+  <si>
+    <t>STRINGS FUNCTIONS</t>
+  </si>
+  <si>
+    <t>// CONCAT</t>
+  </si>
+  <si>
+    <t>CONCAT(COLUMN, " ", ANOTHER_COLUMN)</t>
+  </si>
+  <si>
+    <t>CONCAT_WS(' - ' , COLUMN, ANOTHER_COLUMN)</t>
+  </si>
+  <si>
+    <t>// SUBSTRING</t>
+  </si>
+  <si>
+    <t>SUBSTRING("TEXT", 1, 2)</t>
+  </si>
+  <si>
+    <t>SUBSTRING("TEXT", 2)</t>
+  </si>
+  <si>
+    <t>SUBSTRING("TEXT", -2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// SUBSTR </t>
+  </si>
+  <si>
+    <t>SUBSTR("TEXT", 2)</t>
+  </si>
+  <si>
+    <t>// REPLACE (case-sentitive)</t>
+  </si>
+  <si>
+    <t>REPLACE("ACTUAL WORD", "WHICH WORD", "NEW WORD")</t>
+  </si>
+  <si>
+    <t>// REVERSE</t>
+  </si>
+  <si>
+    <t>REVERSE('TEXT')</t>
+  </si>
+  <si>
+    <t>// CHAR LENGTH</t>
+  </si>
+  <si>
+    <t>CHAR_LENGTH('TEXT')</t>
+  </si>
+  <si>
+    <t>// UPPER-LOWER CASE</t>
+  </si>
+  <si>
+    <t>UPPER('TEXT')</t>
+  </si>
+  <si>
+    <t>LOWER('TEXT')</t>
   </si>
 </sst>
 </file>
@@ -325,12 +382,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -392,19 +449,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -447,59 +491,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,402 +865,539 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J41"/>
+  <dimension ref="B2:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="78.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="85.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="78.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="83.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="85.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="4"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="31" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="G5" s="5" t="s">
+      <c r="E6" s="14"/>
+      <c r="G6" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="20" t="s">
+    <row r="7" spans="2:10">
+      <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="G6" s="5" t="s">
+      <c r="E7" s="14"/>
+      <c r="G7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="8"/>
-      <c r="D7" s="2" t="s">
+    <row r="8" spans="2:10">
+      <c r="B8" s="17"/>
+      <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="G7" s="27" t="s">
+      <c r="E8" s="14"/>
+      <c r="G8" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="7" t="s">
+    <row r="9" spans="2:10">
+      <c r="B9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="G8" s="27" t="s">
+      <c r="E9" s="14"/>
+      <c r="G9" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="20" t="s">
+    <row r="10" spans="2:10">
+      <c r="B10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="G9" s="27" t="s">
+      <c r="E10" s="14"/>
+      <c r="G10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="8"/>
-      <c r="D10" s="24" t="s">
+    <row r="11" spans="2:10">
+      <c r="B11" s="17"/>
+      <c r="D11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="G10" s="27" t="s">
+      <c r="E11" s="14"/>
+      <c r="G11" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="2:10">
+      <c r="B12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="20" t="s">
+      <c r="E12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="I12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="24" t="s">
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="G12" s="5" t="s">
+      <c r="D13" s="20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="8"/>
-      <c r="D13" s="26" t="s">
+      <c r="E13" s="14"/>
+      <c r="G13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="G13" s="27" t="s">
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="17"/>
+      <c r="D14" s="21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="7" t="s">
+      <c r="E14" s="14"/>
+      <c r="G14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="2" t="s">
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="20" t="s">
+      <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="E15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="8"/>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="17"/>
+      <c r="D17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="E17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="E18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="18"/>
-      <c r="E19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="D19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="B20" s="22"/>
+      <c r="E20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="21" t="s">
+      <c r="D21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="25" t="s">
+      <c r="E21" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="29" t="s">
+      <c r="E22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="30" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="30" t="s">
+      <c r="E26" s="28"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" s="7" t="s">
+      <c r="H26" s="28"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="7" t="s">
+      <c r="E28" s="14"/>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D29" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="G26" s="17" t="s">
+      <c r="E29" s="14"/>
+      <c r="G29" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="B27" s="7" t="s">
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D30" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="G27" s="2" t="s">
+      <c r="E30" s="14"/>
+      <c r="G30" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="B28" s="20" t="s">
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D31" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="G28" s="24" t="s">
+      <c r="E31" s="14"/>
+      <c r="G31" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="B29" s="7" t="s">
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D32" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" s="20" t="s">
+      <c r="E32" s="14"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="G30" s="2" t="s">
+      <c r="E33" s="14"/>
+      <c r="G33" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="B31" s="7"/>
-      <c r="E31" s="6"/>
-      <c r="G31" s="24" t="s">
+      <c r="H33" s="14"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="19"/>
+      <c r="E34" s="14"/>
+      <c r="G34" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="2:8">
-      <c r="B32" s="14" t="s">
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="B33" s="7" t="s">
+      <c r="E35" s="14"/>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="2:8">
-      <c r="B34" s="7" t="s">
+      <c r="E36" s="14"/>
+      <c r="H36" s="14"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="B35" s="20" t="s">
+      <c r="E37" s="14"/>
+      <c r="H37" s="14"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="2:8">
-      <c r="B36" s="20" t="s">
+      <c r="E38" s="14"/>
+      <c r="H38" s="14"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="7"/>
-      <c r="E37" s="6"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="14" t="s">
+      <c r="E39" s="14"/>
+      <c r="H39" s="14"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="19"/>
+      <c r="E40" s="14"/>
+      <c r="H40" s="14"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="7" t="s">
+      <c r="E41" s="14"/>
+      <c r="H41" s="14"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="22" t="s">
+      <c r="E42" s="14"/>
+      <c r="H42" s="14"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="15"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="10"/>
+      <c r="E43" s="14"/>
+      <c r="H43" s="14"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="35"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="26"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="9"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="17"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="17"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="17"/>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="17"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="17"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="17"/>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
practise about querying mysql advance concepts
</commit_message>
<xml_diff>
--- a/SQL-Commands.xlsx
+++ b/SQL-Commands.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23313"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2931A1A7-71FD-4E1C-9CA8-2B41112CD492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C061A31-C6CA-4F99-99A9-2CCDF3F0FEE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="111">
   <si>
     <t>SQL Commands</t>
   </si>
@@ -243,58 +244,121 @@
     <t>STRINGS FUNCTIONS</t>
   </si>
   <si>
+    <t>REFINING OUR SELECTIONS</t>
+  </si>
+  <si>
     <t>// CONCAT</t>
   </si>
   <si>
+    <t>// DISTINCT (COMES RIGHT AFTER SELECT)</t>
+  </si>
+  <si>
     <t>CONCAT(COLUMN, " ", ANOTHER_COLUMN)</t>
   </si>
   <si>
+    <t>select distinct &lt;column_nameA&gt;, &lt;column_nameB&gt; from &lt;table_name&gt;;</t>
+  </si>
+  <si>
     <t>CONCAT_WS(' - ' , COLUMN, ANOTHER_COLUMN)</t>
   </si>
   <si>
+    <t>// ORDER BY (ASC By Default), it works with numbers too.</t>
+  </si>
+  <si>
     <t>// SUBSTRING</t>
   </si>
   <si>
+    <t>select &lt;column_nameA&gt; from &lt;table_name&gt;</t>
+  </si>
+  <si>
     <t>SUBSTRING("TEXT", 1, 2)</t>
   </si>
   <si>
+    <t>order by &lt;column_nameA&gt;</t>
+  </si>
+  <si>
     <t>SUBSTRING("TEXT", 2)</t>
   </si>
   <si>
+    <t>(or)</t>
+  </si>
+  <si>
     <t>SUBSTRING("TEXT", -2)</t>
   </si>
   <si>
+    <t>order by &lt;column_nameA&gt; &lt;column_nameB&gt; DESC;</t>
+  </si>
+  <si>
     <t xml:space="preserve">// SUBSTR </t>
   </si>
   <si>
     <t>SUBSTR("TEXT", 2)</t>
   </si>
   <si>
+    <t>order by *2 DESC;</t>
+  </si>
+  <si>
     <t>// REPLACE (case-sentitive)</t>
   </si>
   <si>
+    <t>* No is the column place where we select from!</t>
+  </si>
+  <si>
     <t>REPLACE("ACTUAL WORD", "WHICH WORD", "NEW WORD")</t>
   </si>
   <si>
+    <t>// LIMIT (number)</t>
+  </si>
+  <si>
     <t>// REVERSE</t>
   </si>
   <si>
+    <t xml:space="preserve"># it retrieve first 10 rows </t>
+  </si>
+  <si>
     <t>REVERSE('TEXT')</t>
   </si>
   <si>
+    <t>order by 2 DESC limit 10;</t>
+  </si>
+  <si>
     <t>// CHAR LENGTH</t>
   </si>
   <si>
+    <t>(or) # it retrieve rows from 11th till next 10 rows</t>
+  </si>
+  <si>
     <t>CHAR_LENGTH('TEXT')</t>
   </si>
   <si>
+    <t>order by 2 DESC limit 10, 10;</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; like "%any-letter%"</t>
+  </si>
+  <si>
     <t>// UPPER-LOWER CASE</t>
   </si>
   <si>
     <t>UPPER('TEXT')</t>
   </si>
   <si>
+    <t>// LIKE (WILD CARDS) - % | _ | \</t>
+  </si>
+  <si>
     <t>LOWER('TEXT')</t>
+  </si>
+  <si>
+    <t>select &lt;column_nameA&gt;, &lt;column_nameB&gt; from &lt;table_name&gt;</t>
+  </si>
+  <si>
+    <t>(or) "any-letter%" | "%any-letter" | "%" | "%\%%" | "% %" (it has a space) - This works with texts</t>
+  </si>
+  <si>
+    <t>(or)  _ (1 digit) | __ (2 digits) ....N - This works with numbers</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; like "___"</t>
   </si>
 </sst>
 </file>
@@ -373,7 +437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,12 +446,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -487,27 +557,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,11 +634,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -551,6 +643,22 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,18 +973,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J73"/>
+  <dimension ref="A2:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:B73"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="2.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="78.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="88.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="85.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -889,7 +997,8 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="32"/>
+      <c r="I2" s="33" t="s">
         <v>1</v>
       </c>
     </row>
@@ -897,16 +1006,16 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="8" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -914,32 +1023,32 @@
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="B5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="G6" s="15" t="s">
+      <c r="E6" s="11"/>
+      <c r="G6" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="G7" s="15" t="s">
+      <c r="E7" s="11"/>
+      <c r="G7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -947,36 +1056,36 @@
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="17"/>
-      <c r="D8" s="13" t="s">
+      <c r="B8" s="14"/>
+      <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="G8" s="18" t="s">
+      <c r="E8" s="11"/>
+      <c r="G8" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="G9" s="18" t="s">
+      <c r="E9" s="11"/>
+      <c r="G9" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="G10" s="18" t="s">
+      <c r="E10" s="11"/>
+      <c r="G10" s="15" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -987,417 +1096,508 @@
       </c>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="17"/>
-      <c r="D11" s="20" t="s">
+      <c r="B11" s="14"/>
+      <c r="D11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="G11" s="18" t="s">
+      <c r="E11" s="11"/>
+      <c r="G11" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="E12" s="11"/>
+      <c r="G12" s="12"/>
       <c r="I12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="G13" s="15" t="s">
+      <c r="E13" s="11"/>
+      <c r="G13" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="17"/>
-      <c r="D14" s="21" t="s">
+      <c r="B14" s="14"/>
+      <c r="D14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="G14" s="18" t="s">
+      <c r="E14" s="11"/>
+      <c r="G14" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="E15" s="11"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="17"/>
-      <c r="D17" s="13" t="s">
+      <c r="E16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" s="14"/>
+      <c r="D17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="19" t="s">
+      <c r="E17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="16" t="s">
+      <c r="E18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="B19" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="22"/>
-      <c r="E20" s="14"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="19" t="s">
+      <c r="E19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20" s="19"/>
+      <c r="E20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="B21" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="16" t="s">
+      <c r="E21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="32"/>
+      <c r="B22" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="26"/>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="4" t="s">
+      <c r="E22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="27" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="27" t="s">
+      <c r="E26" s="4"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H26" s="28"/>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="B27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="14"/>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="B28" s="19" t="s">
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="B28" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="H28" s="14"/>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="B29" s="19" t="s">
+      <c r="F28" s="36"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="14"/>
-      <c r="G29" s="31" t="s">
+      <c r="F29" s="36"/>
+      <c r="G29" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" s="19" t="s">
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="14"/>
-      <c r="G30" s="13" t="s">
+      <c r="F30" s="36"/>
+      <c r="G30" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="B31" s="16" t="s">
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="14"/>
-      <c r="G31" s="20" t="s">
+      <c r="F31" s="36"/>
+      <c r="G31" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="H31" s="14"/>
-    </row>
-    <row r="32" spans="2:8">
-      <c r="B32" s="19" t="s">
+    </row>
+    <row r="32" spans="1:7">
+      <c r="B32" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="14"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="14"/>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="B33" s="16" t="s">
+      <c r="F32" s="36"/>
+      <c r="G32" s="38"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="14"/>
-      <c r="G33" s="13" t="s">
+      <c r="F33" s="36"/>
+      <c r="G33" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H33" s="14"/>
-    </row>
-    <row r="34" spans="2:8">
-      <c r="B34" s="19"/>
-      <c r="E34" s="14"/>
-      <c r="G34" s="20" t="s">
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="16"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H34" s="14"/>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="B35" s="33" t="s">
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="14"/>
-      <c r="H35" s="14"/>
-    </row>
-    <row r="36" spans="2:8">
-      <c r="B36" s="19" t="s">
+      <c r="F35" s="36"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="14"/>
-      <c r="H36" s="14"/>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="19" t="s">
+      <c r="F36" s="36"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="H37" s="14"/>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="16" t="s">
+      <c r="F37" s="36"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="H38" s="14"/>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="16" t="s">
+      <c r="F38" s="36"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="14"/>
-      <c r="H39" s="14"/>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="19"/>
-      <c r="E40" s="14"/>
-      <c r="H40" s="14"/>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="33" t="s">
+      <c r="F39" s="36"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="16"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="14"/>
-      <c r="H41" s="14"/>
-    </row>
-    <row r="42" spans="2:8">
-      <c r="B42" s="19" t="s">
+      <c r="F41" s="36"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="H42" s="14"/>
-    </row>
-    <row r="43" spans="2:8">
-      <c r="B43" s="34" t="s">
+      <c r="F42" s="36"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="H43" s="14"/>
-    </row>
-    <row r="44" spans="2:8">
-      <c r="B44" s="35"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="26"/>
-    </row>
-    <row r="47" spans="2:8">
-      <c r="B47" s="4" t="s">
+      <c r="F43" s="36"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="28"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="23"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="48" spans="2:8">
-      <c r="B48" s="9"/>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="19" t="s">
+      <c r="D47" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="34" t="s">
+    <row r="48" spans="2:7">
+      <c r="B48" s="6"/>
+      <c r="D48" s="14"/>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="34" t="s">
+      <c r="D49" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="17"/>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="19" t="s">
+    <row r="50" spans="2:4">
+      <c r="B50" s="27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="34" t="s">
+      <c r="D50" s="27" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="34" t="s">
+    <row r="51" spans="2:4">
+      <c r="B51" s="27" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" s="34" t="s">
+      <c r="D51" s="14"/>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="14"/>
+      <c r="D52" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="17"/>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="19" t="s">
+    <row r="53" spans="2:4">
+      <c r="B53" s="16" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="59" spans="2:2">
-      <c r="B59" s="34" t="s">
+      <c r="D53" s="27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="2:2">
-      <c r="B60" s="17"/>
-    </row>
-    <row r="61" spans="2:2">
-      <c r="B61" s="19" t="s">
+    <row r="54" spans="2:4">
+      <c r="B54" s="27" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="34" t="s">
+      <c r="D54" s="27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="17"/>
-    </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="19" t="s">
+    <row r="55" spans="2:4">
+      <c r="B55" s="27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="34" t="s">
+      <c r="D55" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
-      <c r="B66" s="17"/>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" s="19" t="s">
+    <row r="56" spans="2:4">
+      <c r="B56" s="27" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="34" t="s">
+      <c r="D56" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="14"/>
+      <c r="D57" s="27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="2:2">
-      <c r="B69" s="17"/>
-    </row>
-    <row r="70" spans="2:2">
-      <c r="B70" s="19" t="s">
+    <row r="58" spans="2:4">
+      <c r="B58" s="16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="71" spans="2:2">
-      <c r="B71" s="34" t="s">
+      <c r="D58" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="27" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="72" spans="2:2">
-      <c r="B72" s="34" t="s">
+      <c r="D59" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="14"/>
+      <c r="D60" s="27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="2:2">
-      <c r="B73" s="36"/>
+    <row r="61" spans="2:4">
+      <c r="B61" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="14"/>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" s="14"/>
+      <c r="D63" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" s="14"/>
+      <c r="D66" s="27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="14"/>
+      <c r="D69" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D70" s="27"/>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D71" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="B72" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="B73" s="27"/>
+      <c r="D73" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4">
+      <c r="B74" s="29"/>
+      <c r="D74" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="D75" s="27"/>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="D76" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="D77" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="D78" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="D79" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
learnt about data types advance / aggregate functions in mysql
</commit_message>
<xml_diff>
--- a/SQL-Commands.xlsx
+++ b/SQL-Commands.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23318"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C061A31-C6CA-4F99-99A9-2CCDF3F0FEE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{376BBC0E-9B2F-495C-8D91-CD9C1090EE81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="132">
   <si>
     <t>SQL Commands</t>
   </si>
@@ -247,24 +247,39 @@
     <t>REFINING OUR SELECTIONS</t>
   </si>
   <si>
+    <t>AGGREGATE FUNCTIONS</t>
+  </si>
+  <si>
     <t>// CONCAT</t>
   </si>
   <si>
     <t>// DISTINCT (COMES RIGHT AFTER SELECT)</t>
   </si>
   <si>
+    <t>// count</t>
+  </si>
+  <si>
     <t>CONCAT(COLUMN, " ", ANOTHER_COLUMN)</t>
   </si>
   <si>
     <t>select distinct &lt;column_nameA&gt;, &lt;column_nameB&gt; from &lt;table_name&gt;;</t>
   </si>
   <si>
+    <t>select count(*) from &lt;table_name&gt; where &lt;column_name&gt; like "%...%";</t>
+  </si>
+  <si>
     <t>CONCAT_WS(' - ' , COLUMN, ANOTHER_COLUMN)</t>
   </si>
   <si>
+    <t>select count(&lt;column_nameA&gt;) from &lt;table_name&gt;;</t>
+  </si>
+  <si>
     <t>// ORDER BY (ASC By Default), it works with numbers too.</t>
   </si>
   <si>
+    <t>select count(distinct &lt;column_nameA&gt;, &lt;column_nameB&gt;) from &lt;table_name&gt;;</t>
+  </si>
+  <si>
     <t>// SUBSTRING</t>
   </si>
   <si>
@@ -277,6 +292,9 @@
     <t>order by &lt;column_nameA&gt;</t>
   </si>
   <si>
+    <t>// groupBy</t>
+  </si>
+  <si>
     <t>SUBSTRING("TEXT", 2)</t>
   </si>
   <si>
@@ -286,15 +304,24 @@
     <t>SUBSTRING("TEXT", -2)</t>
   </si>
   <si>
+    <t>group by &lt;column_nameA&gt;</t>
+  </si>
+  <si>
     <t>order by &lt;column_nameA&gt; &lt;column_nameB&gt; DESC;</t>
   </si>
   <si>
     <t xml:space="preserve">// SUBSTR </t>
   </si>
   <si>
+    <t>select &lt;column_nameA&gt;, count(*) from &lt;table_name&gt;</t>
+  </si>
+  <si>
     <t>SUBSTR("TEXT", 2)</t>
   </si>
   <si>
+    <t>group by &lt;column_nameA&gt;, &lt;column_nameB&gt;</t>
+  </si>
+  <si>
     <t>order by *2 DESC;</t>
   </si>
   <si>
@@ -304,12 +331,21 @@
     <t>* No is the column place where we select from!</t>
   </si>
   <si>
+    <t>// min/max/average - IT PRINT OUTS ONE ROW</t>
+  </si>
+  <si>
     <t>REPLACE("ACTUAL WORD", "WHICH WORD", "NEW WORD")</t>
   </si>
   <si>
+    <t>select min(&lt;column_name&gt;) from &lt;table_name&gt;</t>
+  </si>
+  <si>
     <t>// LIMIT (number)</t>
   </si>
   <si>
+    <t>select max(&lt;column_name&gt;) from &lt;table_name&gt;</t>
+  </si>
+  <si>
     <t>// REVERSE</t>
   </si>
   <si>
@@ -319,24 +355,39 @@
     <t>REVERSE('TEXT')</t>
   </si>
   <si>
+    <t>//  sub Queries - without groupBy :-)</t>
+  </si>
+  <si>
     <t>order by 2 DESC limit 10;</t>
   </si>
   <si>
+    <t>select * from &lt;table_name&gt;</t>
+  </si>
+  <si>
     <t>// CHAR LENGTH</t>
   </si>
   <si>
     <t>(or) # it retrieve rows from 11th till next 10 rows</t>
   </si>
   <si>
+    <t>where &lt;column_name&gt; = (SUB-Query)</t>
+  </si>
+  <si>
     <t>CHAR_LENGTH('TEXT')</t>
   </si>
   <si>
     <t>order by 2 DESC limit 10, 10;</t>
   </si>
   <si>
+    <t xml:space="preserve">(or) </t>
+  </si>
+  <si>
     <t>where &lt;column_nameA&gt; like "%any-letter%"</t>
   </si>
   <si>
+    <t>where &lt;column_name&gt; = (select max(&lt;column_nameA&gt;) from &lt;table_name&gt;)</t>
+  </si>
+  <si>
     <t>// UPPER-LOWER CASE</t>
   </si>
   <si>
@@ -346,6 +397,9 @@
     <t>// LIKE (WILD CARDS) - % | _ | \</t>
   </si>
   <si>
+    <t>order by &lt;column_name&gt; desc limit 1;</t>
+  </si>
+  <si>
     <t>LOWER('TEXT')</t>
   </si>
   <si>
@@ -353,6 +407,15 @@
   </si>
   <si>
     <t>(or) "any-letter%" | "%any-letter" | "%" | "%\%%" | "% %" (it has a space) - This works with texts</t>
+  </si>
+  <si>
+    <t>// sum / average (with 4 decimal count)</t>
+  </si>
+  <si>
+    <t>select sum(&lt;column_name&gt;) from &lt;table_name&gt;</t>
+  </si>
+  <si>
+    <t>select average(&lt;column_name&gt;) from &lt;table_name&gt;</t>
   </si>
   <si>
     <t>(or)  _ (1 digit) | __ (2 digits) ....N - This works with numbers</t>
@@ -604,9 +667,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -631,9 +691,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -643,12 +700,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -659,6 +710,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,7 +1039,7 @@
   <dimension ref="A2:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -997,8 +1060,8 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="29" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1010,12 +1073,12 @@
         <v>2</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="37" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1023,32 +1086,32 @@
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="B5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="G6" s="12" t="s">
+      <c r="E6" s="10"/>
+      <c r="G6" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="G7" s="12" t="s">
+      <c r="E7" s="10"/>
+      <c r="G7" s="11" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1056,36 +1119,36 @@
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="14"/>
-      <c r="D8" s="10" t="s">
+      <c r="B8" s="13"/>
+      <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="G8" s="15" t="s">
+      <c r="E8" s="10"/>
+      <c r="G8" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="G9" s="15" t="s">
+      <c r="E9" s="10"/>
+      <c r="G9" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="G10" s="15" t="s">
+      <c r="E10" s="10"/>
+      <c r="G10" s="14" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1096,289 +1159,289 @@
       </c>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="14"/>
-      <c r="D11" s="17" t="s">
+      <c r="B11" s="13"/>
+      <c r="D11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="G11" s="15" t="s">
+      <c r="E11" s="10"/>
+      <c r="G11" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="G12" s="12"/>
+      <c r="E12" s="10"/>
+      <c r="G12" s="11"/>
       <c r="I12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="G13" s="12" t="s">
+      <c r="E13" s="10"/>
+      <c r="G13" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="14"/>
-      <c r="D14" s="18" t="s">
+      <c r="B14" s="13"/>
+      <c r="D14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="G14" s="15" t="s">
+      <c r="E14" s="10"/>
+      <c r="G14" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="E15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="E16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="14"/>
-      <c r="D17" s="10" t="s">
+      <c r="B17" s="13"/>
+      <c r="D17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="E18" s="10"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="E19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" s="19"/>
-      <c r="E20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="B20" s="18"/>
+      <c r="E20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="E21" s="10"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="32"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="28"/>
+      <c r="B22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="E22" s="10"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="22"/>
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="36" t="s">
         <v>47</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="5" t="s">
+      <c r="F26" s="30"/>
+      <c r="G26" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="B27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="8"/>
+      <c r="B27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="11"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37" t="s">
+      <c r="F29" s="32"/>
+      <c r="G29" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="12" t="s">
+      <c r="F30" s="32"/>
+      <c r="G30" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="15" t="s">
+      <c r="F31" s="32"/>
+      <c r="G31" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="38"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="34"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="12" t="s">
+      <c r="F33" s="32"/>
+      <c r="G33" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="16"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="15" t="s">
+      <c r="B34" s="15"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="11"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="36"/>
-      <c r="G36" s="11"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="11"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="36"/>
-      <c r="G38" s="11"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="36"/>
-      <c r="G39" s="11"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="16"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="11"/>
+      <c r="B40" s="15"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F41" s="36"/>
-      <c r="G41" s="11"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F42" s="36"/>
-      <c r="G42" s="11"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="F43" s="36"/>
-      <c r="G43" s="11"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="28"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="23"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="22"/>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="3" t="s">
@@ -1387,217 +1450,296 @@
       <c r="D47" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="G47" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="6"/>
-      <c r="D48" s="14"/>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="16" t="s">
+      <c r="B48" s="5"/>
+      <c r="D48" s="13"/>
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" s="15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" s="27" t="s">
+      <c r="D49" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="27" t="s">
+      <c r="G49" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="27" t="s">
+    <row r="50" spans="2:7">
+      <c r="B50" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="14"/>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52" s="14"/>
-      <c r="D52" s="16" t="s">
+      <c r="D50" s="25" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="B53" s="16" t="s">
+      <c r="G50" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D53" s="27" t="s">
+    </row>
+    <row r="51" spans="2:7">
+      <c r="B51" s="25" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="54" spans="2:4">
-      <c r="B54" s="27" t="s">
+      <c r="D51" s="13"/>
+      <c r="G51" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="27" t="s">
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52" s="13"/>
+      <c r="D52" s="15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="2:4">
-      <c r="B55" s="27" t="s">
+      <c r="G52" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D55" s="14" t="s">
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" s="15" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="56" spans="2:4">
-      <c r="B56" s="27" t="s">
+      <c r="D53" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="D56" s="27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4">
-      <c r="B57" s="14"/>
-      <c r="D57" s="27" t="s">
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="B54" s="25" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="58" spans="2:4">
-      <c r="B58" s="16" t="s">
+      <c r="D54" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4">
-      <c r="B59" s="27" t="s">
+      <c r="G54" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D59" s="27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4">
-      <c r="B60" s="14"/>
-      <c r="D60" s="27" t="s">
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55" s="25" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="61" spans="2:4">
-      <c r="B61" s="16" t="s">
+      <c r="D55" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="G55" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56" s="25" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="62" spans="2:4">
-      <c r="B62" s="27" t="s">
+      <c r="D56" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G56" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D62" s="14"/>
-    </row>
-    <row r="63" spans="2:4">
-      <c r="B63" s="14"/>
-      <c r="D63" s="16" t="s">
+    </row>
+    <row r="57" spans="2:7">
+      <c r="B57" s="13"/>
+      <c r="D57" s="25" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="64" spans="2:4">
-      <c r="B64" s="16" t="s">
+      <c r="G57" s="13"/>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D58" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G58" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="2:4">
-      <c r="B65" s="27" t="s">
+    <row r="59" spans="2:7">
+      <c r="B59" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D65" s="27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4">
-      <c r="B66" s="14"/>
-      <c r="D66" s="27" t="s">
+      <c r="D59" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G59" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="2:4">
-      <c r="B67" s="16" t="s">
+    <row r="60" spans="2:7">
+      <c r="B60" s="13"/>
+      <c r="D60" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="G60" s="13"/>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="B61" s="15" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="68" spans="2:4">
-      <c r="B68" s="27" t="s">
+      <c r="D61" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="G61" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="2:4">
-      <c r="B69" s="14"/>
-      <c r="D69" s="27" t="s">
+    <row r="62" spans="2:7">
+      <c r="B62" s="25" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="70" spans="2:4">
-      <c r="B70" s="16" t="s">
+      <c r="D62" s="13"/>
+      <c r="G62" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D70" s="27"/>
-    </row>
-    <row r="71" spans="2:4">
-      <c r="B71" s="27" t="s">
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63" s="13"/>
+      <c r="D63" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="G63" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="72" spans="2:4">
-      <c r="B72" s="27" t="s">
+    <row r="64" spans="2:7">
+      <c r="B64" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D72" s="27" t="s">
+      <c r="D64" s="13" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="73" spans="2:4">
-      <c r="B73" s="27"/>
-      <c r="D73" s="14" t="s">
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="B65" s="25" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="74" spans="2:4">
-      <c r="B74" s="29"/>
-      <c r="D74" s="27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4">
-      <c r="D75" s="27"/>
-    </row>
-    <row r="76" spans="2:4">
-      <c r="D76" s="27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4">
-      <c r="D77" s="14" t="s">
+      <c r="D65" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G65" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="2:4">
-      <c r="D78" s="27" t="s">
+    <row r="66" spans="2:7">
+      <c r="B66" s="13"/>
+      <c r="D66" s="25" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="79" spans="2:4">
-      <c r="D79" s="29"/>
+      <c r="G66" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7">
+      <c r="B67" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7">
+      <c r="B68" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7">
+      <c r="B69" s="13"/>
+      <c r="D69" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D70" s="25"/>
+      <c r="G70" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="G72" s="13"/>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="B73" s="25"/>
+      <c r="D73" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74" s="27"/>
+      <c r="D74" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7">
+      <c r="D75" s="25"/>
+      <c r="G75" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7">
+      <c r="D76" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="G76" s="13"/>
+    </row>
+    <row r="77" spans="2:7">
+      <c r="D77" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G77" s="13"/>
+    </row>
+    <row r="78" spans="2:7">
+      <c r="D78" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="G78" s="13"/>
+    </row>
+    <row r="79" spans="2:7">
+      <c r="D79" s="27"/>
+      <c r="G79" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>